<commit_message>
first version of streamlit page
</commit_message>
<xml_diff>
--- a/src/project_time_allocation/task/data/input.xlsx
+++ b/src/project_time_allocation/task/data/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ste\Dev\project-time-allocation\src\project_time_allocation\task\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEEA818-9541-4DE4-87F8-B52B67D1547D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46254AA9-4B34-4840-8F87-7557749335AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workers" sheetId="1" r:id="rId1"/>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1206,7 @@
         <v>19</v>
       </c>
       <c r="C2">
-        <v>12000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>